<commit_message>
Write to Excel file implemented
- detekt rules updated
- KDoc updated
- Cell.setCellValue implemented
- Opening mode for ExcelDB implemented
- ExcelDB.writeData and ExcelDB.writeExcel implemented
- The general extension function extracted
- FieldName renamed to FieldReference
- Unit Tests updated
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestWorkBook.xlsx
+++ b/src/test/resources/data/TestWorkBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoly_Machalik/IdeaProjects/ExcelDB/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B525D109-FE62-FF46-B929-B1B819F67B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9276DA8-AC5C-4648-AAD9-541E617E7F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30980" yWindow="3680" windowWidth="28040" windowHeight="17440" firstSheet="4" activeTab="9" xr2:uid="{CED03663-6978-A447-83FC-BFEEDCC7FC52}"/>
+    <workbookView xWindow="-30980" yWindow="3680" windowWidth="28040" windowHeight="17440" firstSheet="4" activeTab="8" xr2:uid="{CED03663-6978-A447-83FC-BFEEDCC7FC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="UserWithDefault" sheetId="5" r:id="rId6"/>
     <sheet name="UserWithOptional" sheetId="6" r:id="rId7"/>
     <sheet name="EmptyUser" sheetId="7" r:id="rId8"/>
-    <sheet name="UserWithUnsupportedField" sheetId="9" r:id="rId9"/>
-    <sheet name="SpecialCharacters" sheetId="10" r:id="rId10"/>
+    <sheet name="EmptySheet" sheetId="11" r:id="rId9"/>
+    <sheet name="UserWithUnsupportedField" sheetId="9" r:id="rId10"/>
+    <sheet name="SpecialCharacters" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -490,10 +491,61 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0DE10-0730-F042-BDF7-74032E9D5C35}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856997CD-275C-4C43-AD00-8F0EE3B2FC4E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -820,52 +872,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0DE10-0730-F042-BDF7-74032E9D5C35}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1674BDE1-A292-B54B-AC17-E531DF0075E9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Column annotation unit testcase implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestWorkBook.xlsx
+++ b/src/test/resources/data/TestWorkBook.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoly_Machalik/IdeaProjects/ExcelDB/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9276DA8-AC5C-4648-AAD9-541E617E7F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFE7F0E-B8E6-CA46-B7B5-33BA3DA48899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30980" yWindow="3680" windowWidth="28040" windowHeight="17440" firstSheet="4" activeTab="8" xr2:uid="{CED03663-6978-A447-83FC-BFEEDCC7FC52}"/>
+    <workbookView xWindow="-32380" yWindow="2440" windowWidth="28040" windowHeight="17440" firstSheet="3" activeTab="10" xr2:uid="{CED03663-6978-A447-83FC-BFEEDCC7FC52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="2" r:id="rId2"/>
-    <sheet name="BoolAndFormula" sheetId="8" r:id="rId3"/>
-    <sheet name="UserMissingColumn" sheetId="3" r:id="rId4"/>
-    <sheet name="UserNonUniqueColumns" sheetId="4" r:id="rId5"/>
-    <sheet name="UserWithDefault" sheetId="5" r:id="rId6"/>
-    <sheet name="UserWithOptional" sheetId="6" r:id="rId7"/>
-    <sheet name="EmptyUser" sheetId="7" r:id="rId8"/>
-    <sheet name="EmptySheet" sheetId="11" r:id="rId9"/>
-    <sheet name="UserWithUnsupportedField" sheetId="9" r:id="rId10"/>
-    <sheet name="SpecialCharacters" sheetId="10" r:id="rId11"/>
+    <sheet name="User" sheetId="2" r:id="rId1"/>
+    <sheet name="BoolAndFormula" sheetId="8" r:id="rId2"/>
+    <sheet name="UserMissingColumn" sheetId="3" r:id="rId3"/>
+    <sheet name="UserNonUniqueColumns" sheetId="4" r:id="rId4"/>
+    <sheet name="UserWithDefault" sheetId="5" r:id="rId5"/>
+    <sheet name="UserWithOptional" sheetId="6" r:id="rId6"/>
+    <sheet name="EmptyUser" sheetId="7" r:id="rId7"/>
+    <sheet name="EmptySheet" sheetId="11" r:id="rId8"/>
+    <sheet name="UserWithUnsupportedField" sheetId="9" r:id="rId9"/>
+    <sheet name="SpecialCharacters" sheetId="10" r:id="rId10"/>
+    <sheet name="UserWithAnnotations" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>col2 _ ()[]{}</t>
+  </si>
+  <si>
+    <t>fullName</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -161,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -479,48 +482,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DF656C-E87E-C146-B873-001CA4312AC6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0DE10-0730-F042-BDF7-74032E9D5C35}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CC4C3F-D2B8-D44E-A4E2-57770F4C682A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -528,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -541,7 +528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{856997CD-275C-4C43-AD00-8F0EE3B2FC4E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -587,13 +574,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CC4C3F-D2B8-D44E-A4E2-57770F4C682A}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD8C295-0A5B-6648-9303-CA09AA8ACA8A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -602,7 +587,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -634,7 +619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E78734B-5EEE-1342-A315-7E6CD4292B82}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -730,7 +715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825BE9E7-C555-5343-813F-C4698DB9CCD3}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -748,7 +733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFD2B6D-56A4-1F4F-8E5F-4FB338007929}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -772,7 +757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F0EFCB-DB40-CA4A-BCAA-FD62EA57DC93}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -829,7 +814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3F9D9B-1D18-A240-9542-762853F97774}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -850,7 +835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9A5982-83DD-4B41-8568-576ED1331BD5}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -871,14 +856,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1674BDE1-A292-B54B-AC17-E531DF0075E9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E0DE10-0730-F042-BDF7-74032E9D5C35}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Improvements - group name changed - sheetName saved to the cache - date cell supported - LocalTime type supported - CellStyle implemented - for date and time cells - keyColumn column removed from Column annotation - Key annotation implemented - clearCache option for writeDataToWorkbook implemented - autoWidth and autoFilter features are implemented -
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestWorkBook.xlsx
+++ b/src/test/resources/data/TestWorkBook.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Karoly_Machalik/IdeaProjects/ExcelDB/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6FD732-1F37-8649-8462-EE8C60BB7BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFC8EF2-2B30-A940-B5E7-BC4A1AA07357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33380" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{CED03663-6978-A447-83FC-BFEEDCC7FC52}"/>
+    <workbookView xWindow="-31380" yWindow="3500" windowWidth="28040" windowHeight="17440" firstSheet="8" activeTab="16" xr2:uid="{CED03663-6978-A447-83FC-BFEEDCC7FC52}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="2" r:id="rId1"/>
@@ -24,15 +24,16 @@
     <sheet name="UserWithUnsupportedField" sheetId="9" r:id="rId9"/>
     <sheet name="SpecialCharacters" sheetId="10" r:id="rId10"/>
     <sheet name="UserWithAnnotations" sheetId="13" r:id="rId11"/>
-    <sheet name="CarFactory" sheetId="15" r:id="rId13"/>
-    <sheet name="CarWithEngine" sheetId="17" r:id="rId14"/>
-    <sheet name="CarNotValidFactory" sheetId="18" r:id="rId15"/>
-    <sheet name="CarNullKey" sheetId="19" r:id="rId16"/>
-    <sheet name="Car" r:id="rId20" sheetId="20"/>
+    <sheet name="CarFactory" sheetId="15" r:id="rId12"/>
+    <sheet name="CarWithEngine" sheetId="17" r:id="rId13"/>
+    <sheet name="CarNotValidFactory" sheetId="18" r:id="rId14"/>
+    <sheet name="CarNullKey" sheetId="19" r:id="rId15"/>
+    <sheet name="Car" sheetId="20" r:id="rId16"/>
+    <sheet name="DataTypes" sheetId="21" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -164,13 +165,40 @@
   <si>
     <t>Fiat</t>
   </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>localdate</t>
+  </si>
+  <si>
+    <t>localdatetime</t>
+  </si>
+  <si>
+    <t>localtime</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -210,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -218,6 +246,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -535,39 +566,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CC4C3F-D2B8-D44E-A4E2-57770F4C682A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -586,17 +617,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -604,16 +635,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -631,34 +662,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -667,7 +698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7281EEC0-A4B2-5543-9625-409AA404BF01}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -676,34 +707,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -712,7 +743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE305A3-FD16-8B4A-9392-618B9CB3BB9C}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -721,66 +752,66 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -789,7 +820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D24AC0-2A65-A64F-9C02-08CF7EAB8A33}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -800,57 +831,57 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>500</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -859,7 +890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8957492C-68E2-C442-A68B-BBD3FDD1DDAD}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -868,55 +899,227 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8BC90C-2A13-F141-89D4-3FF472018157}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45291.999988425923</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45291</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6">
+        <v>45079</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45291.999988425923</v>
+      </c>
+      <c r="I2" s="7">
+        <v>25569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45291.999988425923</v>
+      </c>
+      <c r="D3" s="6">
+        <v>73050</v>
+      </c>
+      <c r="E3">
+        <v>25.2</v>
+      </c>
+      <c r="F3">
+        <v>123456</v>
+      </c>
+      <c r="G3" s="6">
+        <v>73050</v>
+      </c>
+      <c r="H3" s="5">
+        <v>45291.999988425923</v>
+      </c>
+      <c r="I3" s="7">
+        <v>25569.999988425927</v>
       </c>
     </row>
   </sheetData>
@@ -928,41 +1131,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E78734B-5EEE-1342-A315-7E6CD4292B82}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.83203125"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="17.83203125"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="b" s="0">
+      <c r="A2" t="b">
         <v>0</v>
       </c>
-      <c r="B2" s="0">
+      <c r="B2">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="C2" t="str" s="0">
+      <c r="C2" t="str">
         <f>"A"</f>
         <v>A</v>
       </c>
@@ -974,14 +1179,14 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="b" s="0">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <f>3*2</f>
         <v>6</v>
       </c>
-      <c r="C3" t="str" s="0">
+      <c r="C3" t="str">
         <f>_xlfn.CONCAT(C2,"B")</f>
         <v>AB</v>
       </c>
@@ -993,15 +1198,15 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="b" s="0">
+      <c r="A4" t="b">
         <f>OR(A2,A3)</f>
         <v>1</v>
       </c>
-      <c r="B4" s="0">
+      <c r="B4">
         <f>SUM(B2:B3)</f>
         <v>8</v>
       </c>
-      <c r="C4" t="str" s="0">
+      <c r="C4" t="str">
         <f>LOWER(C3)</f>
         <v>ab</v>
       </c>
@@ -1020,74 +1225,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825BE9E7-C555-5343-813F-C4698DB9CCD3}">
   <dimension ref="A1"/>
@@ -1097,7 +1234,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1115,13 +1252,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1138,25 +1275,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1164,18 +1301,18 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1196,10 +1333,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1217,10 +1354,10 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1250,40 +1387,40 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>